<commit_message>
anda recorrer 2 canciones
probe recorrer hasta 3 canciones de 5 y 10 segundos falta probar si escribe bien hasta 30 segundos nose si tirara algun error falopa
</commit_message>
<xml_diff>
--- a/estadisticas.xlsx
+++ b/estadisticas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom\College\PDS-TPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Desktop\FACULTAD - NO TOCA\4to año\Procesamiento Digital de Señales\PDS-TPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168E7514-079D-4378-B2BA-0DBE3B59B9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684CC502-7C26-4FA7-8D72-D80D7B911879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18765" yWindow="4020" windowWidth="14190" windowHeight="13230" xr2:uid="{33177C04-7548-4FEA-A375-AFC23043BE8D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{33177C04-7548-4FEA-A375-AFC23043BE8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
   <si>
     <t>Cancion</t>
   </si>
@@ -60,13 +60,16 @@
     <t>BPM detectado</t>
   </si>
   <si>
+    <t>Tiempo empleado</t>
+  </si>
+  <si>
+    <t>Sin aproximacion inicial</t>
+  </si>
+  <si>
     <t>Con aproximacion inicial</t>
   </si>
   <si>
-    <t>Tiempo empleado</t>
-  </si>
-  <si>
-    <t>Sin aproximacion inicial</t>
+    <t>Bad Bunny - Otra Noche en Miami90BPM.mp3</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -419,160 +422,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A18AEF8-BD3D-43E6-B2E4-148F8B2DCA4D}">
-  <dimension ref="B2:AN4"/>
+  <dimension ref="B1:AN5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AN5" sqref="AN5"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="28" width="21.88671875" customWidth="1"/>
+    <col min="29" max="40" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1" t="s">
+    <row r="1" spans="2:40">
+      <c r="B1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I1" t="n">
+        <v>5</v>
+      </c>
+      <c r="K1" t="n">
+        <v>6</v>
+      </c>
+      <c r="L1" t="n">
+        <v>7</v>
+      </c>
+      <c r="N1" t="n">
+        <v>8</v>
+      </c>
+      <c r="O1" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>10</v>
+      </c>
+      <c r="R1" t="n">
+        <v>11</v>
+      </c>
+      <c r="T1" t="n">
+        <v>12</v>
+      </c>
+      <c r="U1" t="n">
         <v>13</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
+      <c r="W1" t="n">
+        <v>14</v>
+      </c>
+      <c r="X1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AF1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AJ1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AL1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AM1" t="n">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="E3" s="1" t="s">
+    <row r="2" spans="2:40">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="K2" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1" t="s">
+      <c r="Q2" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
+      <c r="W2" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1" t="s">
+      <c r="AC2" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1" t="s">
+      <c r="AI2" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
     </row>
-    <row r="4" spans="2:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:40">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:40">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -586,128 +587,183 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="N4" t="s">
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="P4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Q4" t="s">
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="T4" t="s">
         <v>10</v>
       </c>
       <c r="U4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="V4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="W4" t="s">
         <v>10</v>
       </c>
       <c r="X4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Y4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Z4" t="s">
         <v>10</v>
       </c>
       <c r="AA4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AB4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="AC4" t="s">
         <v>10</v>
       </c>
       <c r="AD4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AE4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="AF4" t="s">
         <v>10</v>
       </c>
       <c r="AG4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AH4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="AI4" t="s">
         <v>10</v>
       </c>
       <c r="AJ4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AK4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="AL4" t="s">
         <v>10</v>
       </c>
       <c r="AM4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="AN4" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:40">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="n">
+        <v>92</v>
+      </c>
+      <c r="F5" t="n">
+        <v>37.4292080402374</v>
+      </c>
+      <c r="H5" t="n">
+        <v>92</v>
+      </c>
+      <c r="I5" t="n">
+        <v>20.4602301120758</v>
+      </c>
+      <c r="K5" t="n">
+        <v>90</v>
+      </c>
+      <c r="L5" t="n">
+        <v>133.327968120575</v>
+      </c>
+      <c r="N5" t="n">
+        <v>90</v>
+      </c>
+      <c r="O5" t="n">
+        <v>60.2935721874237</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>90</v>
+      </c>
+      <c r="R5" t="n">
+        <v>246.002358198166</v>
+      </c>
+      <c r="T5" t="n">
+        <v>90</v>
+      </c>
+      <c r="U5" t="n">
+        <v>79.5626890659332</v>
+      </c>
+      <c r="W5" t="n">
+        <v>90</v>
+      </c>
+      <c r="X5" t="n">
+        <v>396.699867963791</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="W2:AN2"/>
+  <mergeCells count="18">
+    <mergeCell ref="AI2:AN2"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="K2:P2"/>
+    <mergeCell ref="Q2:V2"/>
+    <mergeCell ref="W2:AB2"/>
+    <mergeCell ref="AC2:AH2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="AL3:AN3"/>
     <mergeCell ref="W3:Y3"/>
     <mergeCell ref="Z3:AB3"/>
     <mergeCell ref="AC3:AE3"/>
     <mergeCell ref="AF3:AH3"/>
     <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="E2:V2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>